<commit_message>
Load in next block for route and switch options parameters in line load function
</commit_message>
<xml_diff>
--- a/system_data/lines/green_line.xlsx
+++ b/system_data/lines/green_line.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/system_data/tracks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/system_data/lines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FF3AB56-5112-497A-8217-28F94E7C8719}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA5F5CCE-3E05-41DB-875A-3EB3434447AC}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="0" windowWidth="19410" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19305" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -321,13 +321,13 @@
     <t>84, 86</t>
   </si>
   <si>
-    <t>Initial Next Block</t>
-  </si>
-  <si>
     <t>86, 100</t>
   </si>
   <si>
     <t>29, 30, 149</t>
+  </si>
+  <si>
+    <t>Initial Next Blocks</t>
   </si>
 </sst>
 </file>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I101" sqref="I101"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -745,7 +745,7 @@
         <v>85</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>67</v>
@@ -4412,7 +4412,7 @@
         <v>33</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I86" s="3" t="s">
         <v>97</v>
@@ -7198,7 +7198,7 @@
         <v>20</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I151" s="3">
         <v>29</v>

</xml_diff>

<commit_message>
Updated Excel file with Crossings, default switch positions and lights
</commit_message>
<xml_diff>
--- a/system_data/lines/green_line.xlsx
+++ b/system_data/lines/green_line.xlsx
@@ -5,27 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/system_data/lines/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isabella\Trains\train_system\system_data\lines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA5F5CCE-3E05-41DB-875A-3EB3434447AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448FB28F-EA6D-4A7A-9007-51DBB235B730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="107">
   <si>
     <t>Section</t>
   </si>
@@ -328,6 +339,24 @@
   </si>
   <si>
     <t>Initial Next Blocks</t>
+  </si>
+  <si>
+    <t>Railway Crossing</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Switch Position</t>
+  </si>
+  <si>
+    <t>Light Signal</t>
+  </si>
+  <si>
+    <t>True</t>
   </si>
 </sst>
 </file>
@@ -337,7 +366,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +403,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF2B91AF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -395,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -421,6 +456,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,25 +743,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O154"/>
+  <dimension ref="A1:R154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.54296875" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="13.81640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="23.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="13.77734375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="23.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.21875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="32.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -765,8 +808,17 @@
       <c r="O1" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>42</v>
       </c>
@@ -787,6 +839,9 @@
       </c>
       <c r="G2" s="3" t="s">
         <v>79</v>
+      </c>
+      <c r="H2" s="3">
+        <v>13</v>
       </c>
       <c r="I2" s="3">
         <v>13</v>
@@ -803,8 +858,17 @@
         <f t="shared" ref="O2:O33" si="1">D2*(1/(F2*1000/(60*60)))</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Green</v>
@@ -853,8 +917,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P3" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A67" si="3">A3</f>
         <v>Green</v>
@@ -894,8 +967,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -935,8 +1017,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -976,8 +1067,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P6" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1017,8 +1117,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P7" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1059,8 +1168,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1100,8 +1218,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P9" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1150,8 +1277,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P10" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1191,8 +1327,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P11" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R11" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1232,8 +1377,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P12" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1255,6 +1409,9 @@
       </c>
       <c r="G13" s="3" t="s">
         <v>80</v>
+      </c>
+      <c r="H13" s="3">
+        <v>13</v>
       </c>
       <c r="I13" s="4">
         <f t="shared" si="4"/>
@@ -1275,8 +1432,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P13" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q13" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1317,8 +1483,17 @@
         <f t="shared" si="1"/>
         <v>7.7142857142857153</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P14" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R14" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1358,8 +1533,17 @@
         <f t="shared" si="1"/>
         <v>7.7142857142857153</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P15" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q15" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R15" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1399,8 +1583,17 @@
         <f t="shared" si="1"/>
         <v>7.7142857142857153</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P16" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1449,8 +1642,17 @@
         <f t="shared" si="1"/>
         <v>7.7142857142857153</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P17" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q17" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R17" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1490,8 +1692,17 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P18" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q18" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R18" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1531,8 +1742,17 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P19" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q19" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R19" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1575,8 +1795,17 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P20" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q20" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="R20" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1616,8 +1845,17 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P21" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q21" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R21" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1657,8 +1895,17 @@
         <f t="shared" si="1"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1707,8 +1954,17 @@
         <f t="shared" si="1"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R23" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1748,8 +2004,17 @@
         <f t="shared" si="1"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R24" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1789,8 +2054,17 @@
         <f t="shared" si="1"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R25" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1830,8 +2104,17 @@
         <f t="shared" si="1"/>
         <v>10.285714285714286</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R26" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1871,8 +2154,17 @@
         <f t="shared" si="1"/>
         <v>5.1428571428571432</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R27" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1912,8 +2204,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R28" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1953,8 +2254,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R29" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1998,8 +2308,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q30" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R30" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2021,6 +2340,9 @@
       </c>
       <c r="G31" s="3" t="s">
         <v>88</v>
+      </c>
+      <c r="H31" s="3">
+        <v>30</v>
       </c>
       <c r="I31" s="3">
         <f>C32</f>
@@ -2038,8 +2360,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q31" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R31" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2088,8 +2419,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R32" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2129,8 +2469,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P33" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q33" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R33" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2170,8 +2519,17 @@
         <f t="shared" ref="O34:O65" si="11">D34*(1/(F34*1000/(60*60)))</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P34" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q34" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R34" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2211,8 +2569,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P35" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q35" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R35" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2252,8 +2619,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P36" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q36" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R36" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2296,8 +2672,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P37" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q37" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R37" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Green</v>
@@ -2340,8 +2725,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P38" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q38" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R38" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2384,8 +2778,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P39" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q39" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R39" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2434,8 +2837,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P40" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q40" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R40" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2478,8 +2890,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P41" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q41" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R41" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2522,8 +2943,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P42" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q42" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R42" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2566,8 +2996,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P43" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q43" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R43" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2610,8 +3049,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P44" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q44" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R44" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2654,8 +3102,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P45" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q45" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R45" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2698,8 +3155,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P46" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q46" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R46" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2742,8 +3208,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P47" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q47" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R47" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2786,8 +3261,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P48" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q48" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R48" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2836,8 +3320,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P49" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q49" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R49" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2880,8 +3373,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P50" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q50" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R50" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2924,8 +3426,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P51" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q51" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R51" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2968,8 +3479,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P52" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q52" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R52" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3012,8 +3532,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P53" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q53" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R53" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3056,8 +3585,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P54" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q54" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R54" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3100,8 +3638,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P55" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q55" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R55" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3144,8 +3691,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P56" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q56" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R56" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3188,8 +3744,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P57" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q57" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R57" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3241,8 +3806,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P58" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q58" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R58" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3266,6 +3840,9 @@
         <f t="shared" si="8"/>
         <v>57, 59</v>
       </c>
+      <c r="H59" s="3">
+        <v>57</v>
+      </c>
       <c r="I59" s="3">
         <f t="shared" si="9"/>
         <v>59</v>
@@ -3285,8 +3862,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P59" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q59" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R59" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3326,8 +3912,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P60" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>102</v>
+      </c>
+      <c r="R60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3367,8 +3962,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P61" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q61" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R61" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3408,8 +4012,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P62" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q62" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R62" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3433,6 +4046,9 @@
         <f t="shared" si="8"/>
         <v>61, 63</v>
       </c>
+      <c r="H63" s="3">
+        <v>63</v>
+      </c>
       <c r="I63" s="3">
         <f t="shared" si="9"/>
         <v>63</v>
@@ -3452,8 +4068,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P63" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q63" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R63" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3496,8 +4121,17 @@
         <f t="shared" si="11"/>
         <v>5.1428571428571432</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P64" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q64" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3537,8 +4171,17 @@
         <f t="shared" si="11"/>
         <v>5.1428571428571432</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P65" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>102</v>
+      </c>
+      <c r="R65" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3587,8 +4230,17 @@
         <f t="shared" ref="O66:O97" si="13">D66*(1/(F66*1000/(60*60)))</f>
         <v>10.285714285714286</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P66" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q66" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R66" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3628,8 +4280,17 @@
         <f t="shared" si="13"/>
         <v>10.285714285714286</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P67" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>102</v>
+      </c>
+      <c r="R67" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="str">
         <f t="shared" ref="A68:A131" si="14">A67</f>
         <v>Green</v>
@@ -3669,8 +4330,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P68" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>102</v>
+      </c>
+      <c r="R68" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3710,8 +4380,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P69" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>102</v>
+      </c>
+      <c r="R69" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3751,8 +4430,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P70" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>102</v>
+      </c>
+      <c r="R70" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3792,8 +4480,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P71" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>102</v>
+      </c>
+      <c r="R71" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3833,8 +4530,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P72" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>102</v>
+      </c>
+      <c r="R72" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3874,8 +4580,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P73" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>102</v>
+      </c>
+      <c r="R73" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3924,8 +4639,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P74" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>102</v>
+      </c>
+      <c r="R74" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3965,8 +4689,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P75" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>102</v>
+      </c>
+      <c r="R75" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4006,8 +4739,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P76" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>102</v>
+      </c>
+      <c r="R76" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4029,6 +4771,9 @@
       </c>
       <c r="G77" s="3" t="s">
         <v>81</v>
+      </c>
+      <c r="H77" s="3">
+        <v>77</v>
       </c>
       <c r="I77" s="3">
         <f t="shared" si="9"/>
@@ -4049,8 +4794,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P77" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q77" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="R77" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4100,8 +4854,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P78" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q78" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="R78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4141,8 +4904,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P79" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R79" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4182,8 +4954,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P80" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>102</v>
+      </c>
+      <c r="R80" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4223,8 +5004,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P81" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>102</v>
+      </c>
+      <c r="R81" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4264,8 +5054,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P82" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>102</v>
+      </c>
+      <c r="R82" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4305,8 +5104,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P83" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>102</v>
+      </c>
+      <c r="R83" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4346,8 +5154,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P84" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>102</v>
+      </c>
+      <c r="R84" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4387,8 +5204,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P85" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>102</v>
+      </c>
+      <c r="R85" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4432,8 +5258,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P86" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q86" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="R86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4455,6 +5290,9 @@
       </c>
       <c r="G87" s="3" t="s">
         <v>82</v>
+      </c>
+      <c r="H87" s="3">
+        <v>85</v>
       </c>
       <c r="I87" s="3">
         <f>C88</f>
@@ -4472,8 +5310,17 @@
         <f t="shared" si="13"/>
         <v>14.399999999999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P87" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q87" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="R87" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4513,8 +5360,17 @@
         <f t="shared" si="13"/>
         <v>12.470399999999998</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P88" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>102</v>
+      </c>
+      <c r="R88" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4560,8 +5416,17 @@
         <f t="shared" si="13"/>
         <v>14.399999999999999</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P89" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>102</v>
+      </c>
+      <c r="R89" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4601,8 +5466,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P90" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>102</v>
+      </c>
+      <c r="R90" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4642,8 +5516,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P91" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>102</v>
+      </c>
+      <c r="R91" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4683,8 +5566,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P92" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>102</v>
+      </c>
+      <c r="R92" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4724,8 +5616,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P93" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>102</v>
+      </c>
+      <c r="R93" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4765,8 +5666,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P94" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>102</v>
+      </c>
+      <c r="R94" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4806,8 +5716,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P95" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>102</v>
+      </c>
+      <c r="R95" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4847,8 +5766,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P96" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>102</v>
+      </c>
+      <c r="R96" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4897,8 +5825,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P97" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>102</v>
+      </c>
+      <c r="R97" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4938,8 +5875,17 @@
         <f t="shared" ref="O98:O129" si="21">D98*(1/(F98*1000/(60*60)))</f>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P98" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>102</v>
+      </c>
+      <c r="R98" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4979,8 +5925,17 @@
         <f t="shared" si="21"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P99" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>102</v>
+      </c>
+      <c r="R99" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5020,8 +5975,17 @@
         <f t="shared" si="21"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P100" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>102</v>
+      </c>
+      <c r="R100" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5043,6 +6007,9 @@
       </c>
       <c r="G101" s="3" t="s">
         <v>83</v>
+      </c>
+      <c r="H101" s="3">
+        <v>85</v>
       </c>
       <c r="I101" s="3">
         <v>85</v>
@@ -5059,8 +6026,17 @@
         <f t="shared" si="21"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P101" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q101" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="R101" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5082,6 +6058,9 @@
       </c>
       <c r="G102" s="3" t="s">
         <v>84</v>
+      </c>
+      <c r="H102" s="3">
+        <v>77</v>
       </c>
       <c r="I102" s="3">
         <f t="shared" si="19"/>
@@ -5099,8 +6078,17 @@
         <f t="shared" si="21"/>
         <v>4.8461538461538467</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P102" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q102" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="R102" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5140,8 +6128,17 @@
         <f t="shared" si="21"/>
         <v>12.857142857142859</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P103" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>102</v>
+      </c>
+      <c r="R103" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5181,8 +6178,17 @@
         <f t="shared" si="21"/>
         <v>12.857142857142859</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P104" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>102</v>
+      </c>
+      <c r="R104" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5222,8 +6228,17 @@
         <f t="shared" si="21"/>
         <v>10.285714285714286</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P105" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>102</v>
+      </c>
+      <c r="R105" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5273,8 +6288,17 @@
         <f t="shared" si="21"/>
         <v>12.857142857142859</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P106" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>102</v>
+      </c>
+      <c r="R106" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5314,8 +6338,17 @@
         <f t="shared" si="21"/>
         <v>12.857142857142859</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P107" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>102</v>
+      </c>
+      <c r="R107" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5355,8 +6388,17 @@
         <f t="shared" si="21"/>
         <v>11.571428571428573</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P108" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>102</v>
+      </c>
+      <c r="R108" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5396,8 +6438,17 @@
         <f t="shared" si="21"/>
         <v>12.857142857142859</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P109" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>102</v>
+      </c>
+      <c r="R109" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5437,8 +6488,17 @@
         <f t="shared" si="21"/>
         <v>12.857142857142859</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P110" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>102</v>
+      </c>
+      <c r="R110" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5478,8 +6538,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P111" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>102</v>
+      </c>
+      <c r="R111" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5519,8 +6588,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P112" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q112" t="s">
+        <v>102</v>
+      </c>
+      <c r="R112" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5560,8 +6638,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P113" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>102</v>
+      </c>
+      <c r="R113" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5601,8 +6688,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P114" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>102</v>
+      </c>
+      <c r="R114" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5653,8 +6749,17 @@
         <f t="shared" si="21"/>
         <v>19.439999999999998</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P115" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>102</v>
+      </c>
+      <c r="R115" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5694,8 +6799,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P116" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>102</v>
+      </c>
+      <c r="R116" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5735,8 +6849,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P117" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>102</v>
+      </c>
+      <c r="R117" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5776,8 +6899,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P118" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>102</v>
+      </c>
+      <c r="R118" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5817,8 +6949,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P119" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>102</v>
+      </c>
+      <c r="R119" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5858,8 +6999,17 @@
         <f t="shared" si="21"/>
         <v>9.6</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P120" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>102</v>
+      </c>
+      <c r="R120" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5899,8 +7049,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P121" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>102</v>
+      </c>
+      <c r="R121" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5940,8 +7099,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P122" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>102</v>
+      </c>
+      <c r="R122" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5984,8 +7152,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P123" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>102</v>
+      </c>
+      <c r="R123" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6035,8 +7212,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P124" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>102</v>
+      </c>
+      <c r="R124" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6079,8 +7265,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P125" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>102</v>
+      </c>
+      <c r="R125" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6123,8 +7318,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P126" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q126" t="s">
+        <v>102</v>
+      </c>
+      <c r="R126" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6167,8 +7371,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P127" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>102</v>
+      </c>
+      <c r="R127" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6211,8 +7424,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P128" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q128" t="s">
+        <v>102</v>
+      </c>
+      <c r="R128" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6255,8 +7477,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P129" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q129" t="s">
+        <v>102</v>
+      </c>
+      <c r="R129" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6299,8 +7530,17 @@
         <f t="shared" ref="O130:O151" si="24">D130*(1/(F130*1000/(60*60)))</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P130" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q130" t="s">
+        <v>102</v>
+      </c>
+      <c r="R130" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6343,8 +7583,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P131" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q131" t="s">
+        <v>102</v>
+      </c>
+      <c r="R131" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="str">
         <f t="shared" ref="A132:A151" si="25">A131</f>
         <v>Green</v>
@@ -6387,8 +7636,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="133" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P132" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>102</v>
+      </c>
+      <c r="R132" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6438,8 +7696,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P133" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>102</v>
+      </c>
+      <c r="R133" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6482,8 +7749,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P134" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q134" t="s">
+        <v>102</v>
+      </c>
+      <c r="R134" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6526,8 +7802,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P135" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q135" t="s">
+        <v>102</v>
+      </c>
+      <c r="R135" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6570,8 +7855,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P136" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q136" t="s">
+        <v>102</v>
+      </c>
+      <c r="R136" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6614,8 +7908,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P137" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>102</v>
+      </c>
+      <c r="R137" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6658,8 +7961,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P138" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q138" t="s">
+        <v>102</v>
+      </c>
+      <c r="R138" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6702,8 +8014,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P139" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q139" t="s">
+        <v>102</v>
+      </c>
+      <c r="R139" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6746,8 +8067,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P140" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q140" t="s">
+        <v>102</v>
+      </c>
+      <c r="R140" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6790,8 +8120,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="142" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P141" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q141" t="s">
+        <v>102</v>
+      </c>
+      <c r="R141" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6841,8 +8180,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P142" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q142" t="s">
+        <v>102</v>
+      </c>
+      <c r="R142" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6885,8 +8233,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P143" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q143" t="s">
+        <v>102</v>
+      </c>
+      <c r="R143" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6929,8 +8286,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P144" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>102</v>
+      </c>
+      <c r="R144" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6970,8 +8336,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P145" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>102</v>
+      </c>
+      <c r="R145" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7011,8 +8386,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P146" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q146" t="s">
+        <v>102</v>
+      </c>
+      <c r="R146" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7052,8 +8436,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P147" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q147" t="s">
+        <v>102</v>
+      </c>
+      <c r="R147" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7093,8 +8486,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P148" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q148" t="s">
+        <v>102</v>
+      </c>
+      <c r="R148" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7135,8 +8537,17 @@
         <f t="shared" si="24"/>
         <v>33.119999999999997</v>
       </c>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P149" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q149" t="s">
+        <v>102</v>
+      </c>
+      <c r="R149" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7176,8 +8587,17 @@
         <f t="shared" si="24"/>
         <v>7.1999999999999993</v>
       </c>
-    </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P150" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q150" t="s">
+        <v>102</v>
+      </c>
+      <c r="R150" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7199,6 +8619,9 @@
       </c>
       <c r="G151" s="3" t="s">
         <v>99</v>
+      </c>
+      <c r="H151" s="3">
+        <v>30</v>
       </c>
       <c r="I151" s="3">
         <v>29</v>
@@ -7215,8 +8638,17 @@
         <f t="shared" si="24"/>
         <v>6.3</v>
       </c>
-    </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P151" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q151" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="R151" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A152" s="8" t="s">
         <v>42</v>
       </c>
@@ -7238,6 +8670,9 @@
       <c r="G152" s="3" t="s">
         <v>90</v>
       </c>
+      <c r="H152" s="3">
+        <v>57</v>
+      </c>
       <c r="I152" s="3">
         <v>152</v>
       </c>
@@ -7249,8 +8684,17 @@
         <f t="shared" si="26"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P152" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q152" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="R152" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A153" s="8" t="s">
         <v>42</v>
       </c>
@@ -7283,8 +8727,17 @@
         <f t="shared" si="26"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P153" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q153" t="s">
+        <v>102</v>
+      </c>
+      <c r="R153" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A154" s="8" t="s">
         <v>42</v>
       </c>
@@ -7306,6 +8759,9 @@
       <c r="G154" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="H154" s="3">
+        <v>63</v>
+      </c>
       <c r="I154" s="3">
         <v>63</v>
       </c>
@@ -7316,6 +8772,15 @@
       <c r="N154" s="3">
         <f t="shared" si="26"/>
         <v>0.5</v>
+      </c>
+      <c r="P154" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q154" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="R154" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying to test authority and speed with dipatched train in main
</commit_message>
<xml_diff>
--- a/system_data/lines/green_line.xlsx
+++ b/system_data/lines/green_line.xlsx
@@ -5,20 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/system_data/lines/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/ajb321_pitt_edu/Documents/Documents/Trains/train_system/system_data/lines/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="74" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA5F5CCE-3E05-41DB-875A-3EB3434447AC}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="24285" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -703,23 +714,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="7.54296875" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="13.81640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="23.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="7.53125" customWidth="1"/>
+    <col min="2" max="2" width="9.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.265625" customWidth="1"/>
+    <col min="4" max="4" width="13.19921875" customWidth="1"/>
+    <col min="5" max="5" width="12.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="13.796875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="23.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.19921875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="32.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="32.65" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -766,7 +777,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>42</v>
       </c>
@@ -804,7 +815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Green</v>
@@ -854,7 +865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A67" si="3">A3</f>
         <v>Green</v>
@@ -895,7 +906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -936,7 +947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -977,7 +988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1018,7 +1029,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1060,7 +1071,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1101,7 +1112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1151,7 +1162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1192,7 +1203,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1233,7 +1244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1276,7 +1287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A14" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1318,7 +1329,7 @@
         <v>7.7142857142857153</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A15" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1359,7 +1370,7 @@
         <v>7.7142857142857153</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A16" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1400,7 +1411,7 @@
         <v>7.7142857142857153</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A17" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1450,7 +1461,7 @@
         <v>7.7142857142857153</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A18" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1491,7 +1502,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A19" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1532,7 +1543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A20" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1576,7 +1587,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A21" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1617,7 +1628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A22" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1658,7 +1669,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A23" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1708,7 +1719,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A24" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1749,7 +1760,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A25" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1790,7 +1801,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A26" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1831,7 +1842,7 @@
         <v>10.285714285714286</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A27" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1872,7 +1883,7 @@
         <v>5.1428571428571432</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A28" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1913,7 +1924,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A29" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1954,7 +1965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A30" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1999,7 +2010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A31" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2039,7 +2050,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A32" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2089,7 +2100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A33" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2130,7 +2141,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A34" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2171,7 +2182,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A35" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2212,7 +2223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A36" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2253,7 +2264,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2297,7 +2308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Green</v>
@@ -2341,7 +2352,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A39" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2385,7 +2396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A40" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2435,7 +2446,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A41" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2479,7 +2490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A42" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2523,7 +2534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A43" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2567,7 +2578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A44" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2611,7 +2622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A45" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2655,7 +2666,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A46" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2699,7 +2710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A47" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2743,7 +2754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A48" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2787,7 +2798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A49" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2837,7 +2848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A50" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2881,7 +2892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A51" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2925,7 +2936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A52" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2969,7 +2980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A53" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3013,7 +3024,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A54" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3057,7 +3068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A55" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3101,7 +3112,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A56" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3145,7 +3156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A57" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3189,7 +3200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A58" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3242,7 +3253,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A59" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3286,7 +3297,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A60" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3327,7 +3338,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A61" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3368,7 +3379,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A62" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3409,7 +3420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A63" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3453,7 +3464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A64" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3497,7 +3508,7 @@
         <v>5.1428571428571432</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A65" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3538,7 +3549,7 @@
         <v>5.1428571428571432</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A66" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3588,7 +3599,7 @@
         <v>10.285714285714286</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A67" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3629,7 +3640,7 @@
         <v>10.285714285714286</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A68" s="3" t="str">
         <f t="shared" ref="A68:A131" si="14">A67</f>
         <v>Green</v>
@@ -3670,7 +3681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A69" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3711,7 +3722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A70" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3752,7 +3763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A71" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3793,7 +3804,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A72" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3834,7 +3845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A73" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3875,7 +3886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A74" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3925,7 +3936,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A75" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3966,7 +3977,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A76" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4007,7 +4018,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A77" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4050,7 +4061,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A78" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4101,7 +4112,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A79" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4142,7 +4153,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A80" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4183,7 +4194,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A81" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4224,7 +4235,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A82" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4265,7 +4276,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A83" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4306,7 +4317,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A84" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4347,7 +4358,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A85" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4388,7 +4399,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A86" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4433,7 +4444,7 @@
         <v>15.428571428571431</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A87" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4473,7 +4484,7 @@
         <v>14.399999999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A88" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4514,7 +4525,7 @@
         <v>12.470399999999998</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A89" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4561,7 +4572,7 @@
         <v>14.399999999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A90" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4602,7 +4613,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A91" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4643,7 +4654,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A92" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4684,7 +4695,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A93" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4725,7 +4736,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A94" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4766,7 +4777,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A95" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4807,7 +4818,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A96" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4848,7 +4859,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A97" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4898,7 +4909,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A98" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4939,7 +4950,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A99" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4980,7 +4991,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A100" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5021,7 +5032,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A101" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5060,7 +5071,7 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A102" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5100,7 +5111,7 @@
         <v>4.8461538461538467</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A103" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5141,7 +5152,7 @@
         <v>12.857142857142859</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A104" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5182,7 +5193,7 @@
         <v>12.857142857142859</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A105" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5223,7 +5234,7 @@
         <v>10.285714285714286</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A106" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5274,7 +5285,7 @@
         <v>12.857142857142859</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A107" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5315,7 +5326,7 @@
         <v>12.857142857142859</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A108" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5356,7 +5367,7 @@
         <v>11.571428571428573</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A109" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5397,7 +5408,7 @@
         <v>12.857142857142859</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A110" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5438,7 +5449,7 @@
         <v>12.857142857142859</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A111" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5479,7 +5490,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A112" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5520,7 +5531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A113" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5561,7 +5572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A114" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5602,7 +5613,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A115" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5654,7 +5665,7 @@
         <v>19.439999999999998</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A116" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5695,7 +5706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A117" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5736,7 +5747,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A118" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5777,7 +5788,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A119" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5818,7 +5829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A120" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5859,7 +5870,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A121" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5900,7 +5911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A122" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5941,7 +5952,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A123" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5985,7 +5996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A124" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6036,7 +6047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A125" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6080,7 +6091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A126" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6124,7 +6135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A127" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6168,7 +6179,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A128" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6212,7 +6223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A129" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6256,7 +6267,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A130" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6300,7 +6311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A131" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6344,7 +6355,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A132" s="3" t="str">
         <f t="shared" ref="A132:A151" si="25">A131</f>
         <v>Green</v>
@@ -6388,7 +6399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A133" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6439,7 +6450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A134" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6483,7 +6494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A135" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6527,7 +6538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A136" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6571,7 +6582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A137" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6615,7 +6626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A138" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6659,7 +6670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A139" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6703,7 +6714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A140" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6747,7 +6758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A141" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6791,7 +6802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A142" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6842,7 +6853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A143" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6886,7 +6897,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A144" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6930,7 +6941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A145" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6971,7 +6982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A146" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7012,7 +7023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A147" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7053,7 +7064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A148" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7094,7 +7105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A149" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7136,7 +7147,7 @@
         <v>33.119999999999997</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A150" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7177,7 +7188,7 @@
         <v>7.1999999999999993</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A151" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7216,7 +7227,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A152" s="8" t="s">
         <v>42</v>
       </c>
@@ -7250,7 +7261,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A153" s="8" t="s">
         <v>42</v>
       </c>
@@ -7284,7 +7295,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A154" s="8" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Updates to excel sheet and PLC code
</commit_message>
<xml_diff>
--- a/system_data/lines/green_line.xlsx
+++ b/system_data/lines/green_line.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isabella\Trains\train_system\system_data\lines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448FB28F-EA6D-4A7A-9007-51DBB235B730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CA821C-5C43-4637-AECD-F8EB609CF3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -862,7 +862,7 @@
         <v>102</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>102</v>
@@ -2312,10 +2312,10 @@
         <v>102</v>
       </c>
       <c r="Q30" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="R30" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -2364,7 +2364,7 @@
         <v>102</v>
       </c>
       <c r="Q31" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="R31" s="9" t="s">
         <v>102</v>
@@ -3810,7 +3810,7 @@
         <v>102</v>
       </c>
       <c r="Q58" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="R58" s="9">
         <v>0</v>
@@ -4125,7 +4125,7 @@
         <v>102</v>
       </c>
       <c r="Q64" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="R64">
         <v>0</v>
@@ -4798,7 +4798,7 @@
         <v>102</v>
       </c>
       <c r="Q77" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="R77" t="s">
         <v>102</v>
@@ -5314,7 +5314,7 @@
         <v>102</v>
       </c>
       <c r="Q87" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="R87" t="s">
         <v>102</v>
@@ -8642,7 +8642,7 @@
         <v>102</v>
       </c>
       <c r="Q151" s="11" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="R151" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
BAD COMMIT. GOING TO PULL FROM MAIN
</commit_message>
<xml_diff>
--- a/system_data/lines/green_line.xlsx
+++ b/system_data/lines/green_line.xlsx
@@ -5,27 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0c4a204f81830ef/Pitt/2024_Summer_Term/ECE 1140/Project/train_system/system_data/lines/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isabella\Trains\train_system\system_data\lines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="11_F25DC773A252ABDACC104823A11D487E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA5F5CCE-3E05-41DB-875A-3EB3434447AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448FB28F-EA6D-4A7A-9007-51DBB235B730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="107">
   <si>
     <t>Section</t>
   </si>
@@ -328,6 +339,24 @@
   </si>
   <si>
     <t>Initial Next Blocks</t>
+  </si>
+  <si>
+    <t>Railway Crossing</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Switch Position</t>
+  </si>
+  <si>
+    <t>Light Signal</t>
+  </si>
+  <si>
+    <t>True</t>
   </si>
 </sst>
 </file>
@@ -337,7 +366,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +403,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF2B91AF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -395,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -421,6 +456,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,25 +743,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O154"/>
+  <dimension ref="A1:R154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.54296875" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="13.81640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="23.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="13.77734375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="23.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.21875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="32.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -765,8 +808,17 @@
       <c r="O1" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>42</v>
       </c>
@@ -787,6 +839,9 @@
       </c>
       <c r="G2" s="3" t="s">
         <v>79</v>
+      </c>
+      <c r="H2" s="3">
+        <v>13</v>
       </c>
       <c r="I2" s="3">
         <v>13</v>
@@ -803,8 +858,17 @@
         <f t="shared" ref="O2:O33" si="1">D2*(1/(F2*1000/(60*60)))</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Green</v>
@@ -853,8 +917,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P3" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A67" si="3">A3</f>
         <v>Green</v>
@@ -894,8 +967,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -935,8 +1017,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -976,8 +1067,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P6" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1017,8 +1117,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P7" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1059,8 +1168,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1100,8 +1218,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P9" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1150,8 +1277,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P10" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1191,8 +1327,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P11" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R11" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1232,8 +1377,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P12" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1255,6 +1409,9 @@
       </c>
       <c r="G13" s="3" t="s">
         <v>80</v>
+      </c>
+      <c r="H13" s="3">
+        <v>13</v>
       </c>
       <c r="I13" s="4">
         <f t="shared" si="4"/>
@@ -1275,8 +1432,17 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P13" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q13" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1317,8 +1483,17 @@
         <f t="shared" si="1"/>
         <v>7.7142857142857153</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P14" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R14" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1358,8 +1533,17 @@
         <f t="shared" si="1"/>
         <v>7.7142857142857153</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P15" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q15" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R15" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1399,8 +1583,17 @@
         <f t="shared" si="1"/>
         <v>7.7142857142857153</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P16" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1449,8 +1642,17 @@
         <f t="shared" si="1"/>
         <v>7.7142857142857153</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P17" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q17" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R17" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1490,8 +1692,17 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P18" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q18" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R18" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1531,8 +1742,17 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P19" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q19" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R19" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1575,8 +1795,17 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P20" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q20" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="R20" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1616,8 +1845,17 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P21" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q21" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R21" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1657,8 +1895,17 @@
         <f t="shared" si="1"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1707,8 +1954,17 @@
         <f t="shared" si="1"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R23" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1748,8 +2004,17 @@
         <f t="shared" si="1"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R24" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1789,8 +2054,17 @@
         <f t="shared" si="1"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R25" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1830,8 +2104,17 @@
         <f t="shared" si="1"/>
         <v>10.285714285714286</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R26" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1871,8 +2154,17 @@
         <f t="shared" si="1"/>
         <v>5.1428571428571432</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R27" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1912,8 +2204,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R28" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1953,8 +2254,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R29" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -1998,8 +2308,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q30" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R30" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2021,6 +2340,9 @@
       </c>
       <c r="G31" s="3" t="s">
         <v>88</v>
+      </c>
+      <c r="H31" s="3">
+        <v>30</v>
       </c>
       <c r="I31" s="3">
         <f>C32</f>
@@ -2038,8 +2360,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q31" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R31" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2088,8 +2419,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R32" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2129,8 +2469,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P33" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q33" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R33" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2170,8 +2519,17 @@
         <f t="shared" ref="O34:O65" si="11">D34*(1/(F34*1000/(60*60)))</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P34" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q34" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R34" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2211,8 +2569,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P35" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q35" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R35" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2252,8 +2619,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P36" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q36" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R36" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2296,8 +2672,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P37" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q37" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R37" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Green</v>
@@ -2340,8 +2725,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P38" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q38" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R38" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2384,8 +2778,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P39" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q39" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R39" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2434,8 +2837,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P40" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q40" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R40" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2478,8 +2890,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P41" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q41" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R41" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2522,8 +2943,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P42" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q42" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R42" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2566,8 +2996,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P43" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q43" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R43" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2610,8 +3049,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P44" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q44" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R44" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2654,8 +3102,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P45" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q45" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R45" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2698,8 +3155,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P46" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q46" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R46" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2742,8 +3208,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P47" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q47" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R47" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2786,8 +3261,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P48" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q48" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R48" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2836,8 +3320,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P49" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q49" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R49" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2880,8 +3373,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P50" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q50" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R50" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2924,8 +3426,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P51" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q51" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R51" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -2968,8 +3479,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P52" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q52" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R52" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3012,8 +3532,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P53" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q53" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R53" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3056,8 +3585,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P54" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q54" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R54" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3100,8 +3638,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P55" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q55" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R55" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3144,8 +3691,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P56" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q56" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R56" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3188,8 +3744,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P57" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q57" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R57" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3241,8 +3806,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P58" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q58" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R58" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3266,6 +3840,9 @@
         <f t="shared" si="8"/>
         <v>57, 59</v>
       </c>
+      <c r="H59" s="3">
+        <v>57</v>
+      </c>
       <c r="I59" s="3">
         <f t="shared" si="9"/>
         <v>59</v>
@@ -3285,8 +3862,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P59" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q59" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R59" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3326,8 +3912,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P60" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>102</v>
+      </c>
+      <c r="R60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3367,8 +3962,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P61" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q61" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R61" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3408,8 +4012,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P62" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q62" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R62" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3433,6 +4046,9 @@
         <f t="shared" si="8"/>
         <v>61, 63</v>
       </c>
+      <c r="H63" s="3">
+        <v>63</v>
+      </c>
       <c r="I63" s="3">
         <f t="shared" si="9"/>
         <v>63</v>
@@ -3452,8 +4068,17 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P63" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q63" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="R63" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3496,8 +4121,17 @@
         <f t="shared" si="11"/>
         <v>5.1428571428571432</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P64" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q64" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3537,8 +4171,17 @@
         <f t="shared" si="11"/>
         <v>5.1428571428571432</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P65" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>102</v>
+      </c>
+      <c r="R65" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3587,8 +4230,17 @@
         <f t="shared" ref="O66:O97" si="13">D66*(1/(F66*1000/(60*60)))</f>
         <v>10.285714285714286</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P66" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q66" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R66" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Green</v>
@@ -3628,8 +4280,17 @@
         <f t="shared" si="13"/>
         <v>10.285714285714286</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P67" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>102</v>
+      </c>
+      <c r="R67" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="str">
         <f t="shared" ref="A68:A131" si="14">A67</f>
         <v>Green</v>
@@ -3669,8 +4330,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P68" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>102</v>
+      </c>
+      <c r="R68" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3710,8 +4380,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P69" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>102</v>
+      </c>
+      <c r="R69" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3751,8 +4430,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P70" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>102</v>
+      </c>
+      <c r="R70" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3792,8 +4480,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P71" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>102</v>
+      </c>
+      <c r="R71" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3833,8 +4530,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P72" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>102</v>
+      </c>
+      <c r="R72" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3874,8 +4580,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P73" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>102</v>
+      </c>
+      <c r="R73" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3924,8 +4639,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P74" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>102</v>
+      </c>
+      <c r="R74" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -3965,8 +4689,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P75" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>102</v>
+      </c>
+      <c r="R75" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4006,8 +4739,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P76" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>102</v>
+      </c>
+      <c r="R76" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4029,6 +4771,9 @@
       </c>
       <c r="G77" s="3" t="s">
         <v>81</v>
+      </c>
+      <c r="H77" s="3">
+        <v>77</v>
       </c>
       <c r="I77" s="3">
         <f t="shared" si="9"/>
@@ -4049,8 +4794,17 @@
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P77" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q77" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="R77" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4100,8 +4854,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P78" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q78" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="R78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4141,8 +4904,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P79" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>102</v>
+      </c>
+      <c r="R79" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4182,8 +4954,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P80" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>102</v>
+      </c>
+      <c r="R80" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4223,8 +5004,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P81" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>102</v>
+      </c>
+      <c r="R81" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4264,8 +5054,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P82" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>102</v>
+      </c>
+      <c r="R82" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4305,8 +5104,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P83" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>102</v>
+      </c>
+      <c r="R83" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4346,8 +5154,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P84" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>102</v>
+      </c>
+      <c r="R84" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4387,8 +5204,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P85" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>102</v>
+      </c>
+      <c r="R85" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4432,8 +5258,17 @@
         <f t="shared" si="13"/>
         <v>15.428571428571431</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P86" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q86" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="R86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4455,6 +5290,9 @@
       </c>
       <c r="G87" s="3" t="s">
         <v>82</v>
+      </c>
+      <c r="H87" s="3">
+        <v>85</v>
       </c>
       <c r="I87" s="3">
         <f>C88</f>
@@ -4472,8 +5310,17 @@
         <f t="shared" si="13"/>
         <v>14.399999999999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P87" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q87" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="R87" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4513,8 +5360,17 @@
         <f t="shared" si="13"/>
         <v>12.470399999999998</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P88" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>102</v>
+      </c>
+      <c r="R88" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4560,8 +5416,17 @@
         <f t="shared" si="13"/>
         <v>14.399999999999999</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P89" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>102</v>
+      </c>
+      <c r="R89" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4601,8 +5466,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P90" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>102</v>
+      </c>
+      <c r="R90" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4642,8 +5516,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P91" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>102</v>
+      </c>
+      <c r="R91" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4683,8 +5566,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P92" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>102</v>
+      </c>
+      <c r="R92" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4724,8 +5616,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P93" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>102</v>
+      </c>
+      <c r="R93" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4765,8 +5666,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P94" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>102</v>
+      </c>
+      <c r="R94" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4806,8 +5716,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P95" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>102</v>
+      </c>
+      <c r="R95" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4847,8 +5766,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P96" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>102</v>
+      </c>
+      <c r="R96" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4897,8 +5825,17 @@
         <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P97" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>102</v>
+      </c>
+      <c r="R97" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4938,8 +5875,17 @@
         <f t="shared" ref="O98:O129" si="21">D98*(1/(F98*1000/(60*60)))</f>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P98" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>102</v>
+      </c>
+      <c r="R98" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -4979,8 +5925,17 @@
         <f t="shared" si="21"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P99" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>102</v>
+      </c>
+      <c r="R99" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5020,8 +5975,17 @@
         <f t="shared" si="21"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P100" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>102</v>
+      </c>
+      <c r="R100" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5043,6 +6007,9 @@
       </c>
       <c r="G101" s="3" t="s">
         <v>83</v>
+      </c>
+      <c r="H101" s="3">
+        <v>85</v>
       </c>
       <c r="I101" s="3">
         <v>85</v>
@@ -5059,8 +6026,17 @@
         <f t="shared" si="21"/>
         <v>10.799999999999999</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P101" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q101" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="R101" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5082,6 +6058,9 @@
       </c>
       <c r="G102" s="3" t="s">
         <v>84</v>
+      </c>
+      <c r="H102" s="3">
+        <v>77</v>
       </c>
       <c r="I102" s="3">
         <f t="shared" si="19"/>
@@ -5099,8 +6078,17 @@
         <f t="shared" si="21"/>
         <v>4.8461538461538467</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P102" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q102" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="R102" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5140,8 +6128,17 @@
         <f t="shared" si="21"/>
         <v>12.857142857142859</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P103" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>102</v>
+      </c>
+      <c r="R103" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5181,8 +6178,17 @@
         <f t="shared" si="21"/>
         <v>12.857142857142859</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P104" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>102</v>
+      </c>
+      <c r="R104" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5222,8 +6228,17 @@
         <f t="shared" si="21"/>
         <v>10.285714285714286</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P105" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>102</v>
+      </c>
+      <c r="R105" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5273,8 +6288,17 @@
         <f t="shared" si="21"/>
         <v>12.857142857142859</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P106" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>102</v>
+      </c>
+      <c r="R106" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5314,8 +6338,17 @@
         <f t="shared" si="21"/>
         <v>12.857142857142859</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P107" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>102</v>
+      </c>
+      <c r="R107" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5355,8 +6388,17 @@
         <f t="shared" si="21"/>
         <v>11.571428571428573</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P108" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>102</v>
+      </c>
+      <c r="R108" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5396,8 +6438,17 @@
         <f t="shared" si="21"/>
         <v>12.857142857142859</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P109" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>102</v>
+      </c>
+      <c r="R109" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5437,8 +6488,17 @@
         <f t="shared" si="21"/>
         <v>12.857142857142859</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P110" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>102</v>
+      </c>
+      <c r="R110" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5478,8 +6538,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P111" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>102</v>
+      </c>
+      <c r="R111" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5519,8 +6588,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P112" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q112" t="s">
+        <v>102</v>
+      </c>
+      <c r="R112" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5560,8 +6638,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P113" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>102</v>
+      </c>
+      <c r="R113" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5601,8 +6688,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P114" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>102</v>
+      </c>
+      <c r="R114" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5653,8 +6749,17 @@
         <f t="shared" si="21"/>
         <v>19.439999999999998</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P115" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>102</v>
+      </c>
+      <c r="R115" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5694,8 +6799,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P116" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>102</v>
+      </c>
+      <c r="R116" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5735,8 +6849,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P117" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>102</v>
+      </c>
+      <c r="R117" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5776,8 +6899,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P118" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>102</v>
+      </c>
+      <c r="R118" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5817,8 +6949,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P119" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>102</v>
+      </c>
+      <c r="R119" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5858,8 +6999,17 @@
         <f t="shared" si="21"/>
         <v>9.6</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P120" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>102</v>
+      </c>
+      <c r="R120" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5899,8 +7049,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P121" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>102</v>
+      </c>
+      <c r="R121" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5940,8 +7099,17 @@
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P122" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>102</v>
+      </c>
+      <c r="R122" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -5984,8 +7152,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P123" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>102</v>
+      </c>
+      <c r="R123" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6035,8 +7212,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P124" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>102</v>
+      </c>
+      <c r="R124" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6079,8 +7265,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P125" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>102</v>
+      </c>
+      <c r="R125" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6123,8 +7318,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P126" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q126" t="s">
+        <v>102</v>
+      </c>
+      <c r="R126" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6167,8 +7371,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P127" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>102</v>
+      </c>
+      <c r="R127" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6211,8 +7424,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P128" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q128" t="s">
+        <v>102</v>
+      </c>
+      <c r="R128" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6255,8 +7477,17 @@
         <f t="shared" si="21"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P129" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q129" t="s">
+        <v>102</v>
+      </c>
+      <c r="R129" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6299,8 +7530,17 @@
         <f t="shared" ref="O130:O151" si="24">D130*(1/(F130*1000/(60*60)))</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P130" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q130" t="s">
+        <v>102</v>
+      </c>
+      <c r="R130" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Green</v>
@@ -6343,8 +7583,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P131" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q131" t="s">
+        <v>102</v>
+      </c>
+      <c r="R131" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="str">
         <f t="shared" ref="A132:A151" si="25">A131</f>
         <v>Green</v>
@@ -6387,8 +7636,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="133" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P132" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>102</v>
+      </c>
+      <c r="R132" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6438,8 +7696,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P133" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>102</v>
+      </c>
+      <c r="R133" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6482,8 +7749,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P134" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q134" t="s">
+        <v>102</v>
+      </c>
+      <c r="R134" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6526,8 +7802,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P135" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q135" t="s">
+        <v>102</v>
+      </c>
+      <c r="R135" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6570,8 +7855,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P136" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q136" t="s">
+        <v>102</v>
+      </c>
+      <c r="R136" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6614,8 +7908,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P137" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>102</v>
+      </c>
+      <c r="R137" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6658,8 +7961,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P138" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q138" t="s">
+        <v>102</v>
+      </c>
+      <c r="R138" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6702,8 +8014,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P139" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q139" t="s">
+        <v>102</v>
+      </c>
+      <c r="R139" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6746,8 +8067,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P140" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q140" t="s">
+        <v>102</v>
+      </c>
+      <c r="R140" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6790,8 +8120,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="142" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="P141" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q141" t="s">
+        <v>102</v>
+      </c>
+      <c r="R141" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6841,8 +8180,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P142" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q142" t="s">
+        <v>102</v>
+      </c>
+      <c r="R142" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6885,8 +8233,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P143" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q143" t="s">
+        <v>102</v>
+      </c>
+      <c r="R143" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6929,8 +8286,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P144" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>102</v>
+      </c>
+      <c r="R144" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -6970,8 +8336,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P145" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>102</v>
+      </c>
+      <c r="R145" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7011,8 +8386,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P146" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q146" t="s">
+        <v>102</v>
+      </c>
+      <c r="R146" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7052,8 +8436,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P147" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q147" t="s">
+        <v>102</v>
+      </c>
+      <c r="R147" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7093,8 +8486,17 @@
         <f t="shared" si="24"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P148" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q148" t="s">
+        <v>102</v>
+      </c>
+      <c r="R148" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7135,8 +8537,17 @@
         <f t="shared" si="24"/>
         <v>33.119999999999997</v>
       </c>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P149" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q149" t="s">
+        <v>102</v>
+      </c>
+      <c r="R149" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7176,8 +8587,17 @@
         <f t="shared" si="24"/>
         <v>7.1999999999999993</v>
       </c>
-    </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P150" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q150" t="s">
+        <v>102</v>
+      </c>
+      <c r="R150" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="str">
         <f t="shared" si="25"/>
         <v>Green</v>
@@ -7199,6 +8619,9 @@
       </c>
       <c r="G151" s="3" t="s">
         <v>99</v>
+      </c>
+      <c r="H151" s="3">
+        <v>30</v>
       </c>
       <c r="I151" s="3">
         <v>29</v>
@@ -7215,8 +8638,17 @@
         <f t="shared" si="24"/>
         <v>6.3</v>
       </c>
-    </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P151" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q151" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="R151" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A152" s="8" t="s">
         <v>42</v>
       </c>
@@ -7238,6 +8670,9 @@
       <c r="G152" s="3" t="s">
         <v>90</v>
       </c>
+      <c r="H152" s="3">
+        <v>57</v>
+      </c>
       <c r="I152" s="3">
         <v>152</v>
       </c>
@@ -7249,8 +8684,17 @@
         <f t="shared" si="26"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P152" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q152" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="R152" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A153" s="8" t="s">
         <v>42</v>
       </c>
@@ -7283,8 +8727,17 @@
         <f t="shared" si="26"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P153" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q153" t="s">
+        <v>102</v>
+      </c>
+      <c r="R153" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A154" s="8" t="s">
         <v>42</v>
       </c>
@@ -7306,6 +8759,9 @@
       <c r="G154" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="H154" s="3">
+        <v>63</v>
+      </c>
       <c r="I154" s="3">
         <v>63</v>
       </c>
@@ -7316,6 +8772,15 @@
       <c r="N154" s="3">
         <f t="shared" si="26"/>
         <v>0.5</v>
+      </c>
+      <c r="P154" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q154" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="R154" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>